<commit_message>
Added code for generating the running report for all exam tabs in the workbook
</commit_message>
<xml_diff>
--- a/VisualizeTest.xlsx
+++ b/VisualizeTest.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\VBA\ReportVisualization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE949B1-E7B2-4A78-B5FB-98C14384AAD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DBB4D7-535F-4DE4-B1B4-A9BCB7F7A272}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{34CDE331-2BE0-4989-A0C3-15C3DC22DD25}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{34CDE331-2BE0-4989-A0C3-15C3DC22DD25}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1 (3)" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1 (4)" sheetId="4" r:id="rId4"/>
+    <sheet name="RunningReport" sheetId="5" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1 (3)" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1 (4)" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$H$132</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sheet1 (2)'!$A$2:$H$132</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Sheet1 (3)'!$A$2:$H$132</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Sheet1 (4)'!$A$2:$H$132</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$2:$H$132</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Sheet1 (2)'!$A$2:$H$132</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Sheet1 (3)'!$A$2:$H$132</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Sheet1 (4)'!$A$2:$H$132</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="92">
   <si>
     <t>PCM2 EXAM4 (BSCE BK3) - PART 1-3</t>
   </si>
@@ -337,6 +338,9 @@
   </si>
   <si>
     <t>% of Total Errors</t>
+  </si>
+  <si>
+    <t>188</t>
   </si>
 </sst>
 </file>
@@ -736,7 +740,10 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
@@ -776,36 +783,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -818,7 +795,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$M$2</c:f>
+              <c:f>RunningReport!$M$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -839,7 +816,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$K$3:$L$13</c:f>
+              <c:f>RunningReport!$K$3:$L$13</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="11"/>
                 <c:lvl>
@@ -917,34 +894,46 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$3:$M$13</c:f>
+              <c:f>RunningReport!$M$3:$M$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2</c:v>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6035-4E7C-95B3-92E88CC10496}"/>
+              <c16:uniqueId val="{00000000-A604-4D5C-ADF5-85AB9A1778D8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -953,7 +942,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$2</c:f>
+              <c:f>RunningReport!$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -974,7 +963,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$K$3:$L$13</c:f>
+              <c:f>RunningReport!$K$3:$L$13</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="11"/>
                 <c:lvl>
@@ -1052,39 +1041,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$3:$N$13</c:f>
+              <c:f>RunningReport!$N$3:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.16</c:v>
+                  <c:v>0.11170212765957446</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32</c:v>
+                  <c:v>0.11170212765957446</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.24</c:v>
+                  <c:v>0.11702127659574468</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.12</c:v>
+                  <c:v>0.11702127659574468</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.12</c:v>
+                  <c:v>0.15425531914893617</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.04</c:v>
+                  <c:v>9.0425531914893623E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>8.5106382978723402E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>8.5106382978723402E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>8.5106382978723402E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>3.7234042553191488E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -1094,7 +1083,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-6035-4E7C-95B3-92E88CC10496}"/>
+              <c16:uniqueId val="{00000001-A604-4D5C-ADF5-85AB9A1778D8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1108,11 +1097,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="668970568"/>
-        <c:axId val="668967288"/>
+        <c:axId val="384143576"/>
+        <c:axId val="384141936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="668970568"/>
+        <c:axId val="384143576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1155,7 +1144,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="668967288"/>
+        <c:crossAx val="384141936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1163,7 +1152,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="668967288"/>
+        <c:axId val="384141936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1214,7 +1203,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="668970568"/>
+        <c:crossAx val="384143576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1226,37 +1215,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1357,7 +1315,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sheet1 (2)'!$M$2</c:f>
+              <c:f>Sheet1!$M$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1378,7 +1336,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Sheet1 (2)'!$K$3:$L$13</c:f>
+              <c:f>Sheet1!$K$3:$L$13</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="11"/>
                 <c:lvl>
@@ -1456,43 +1414,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet1 (2)'!$M$3:$M$13</c:f>
+              <c:f>Sheet1!$M$3:$M$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>14</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6130-4703-A271-EBB8FC5EFE15}"/>
+              <c16:uniqueId val="{00000000-8306-4031-ABC8-1844283DA1A9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1501,7 +1450,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sheet1 (2)'!$N$2</c:f>
+              <c:f>Sheet1!$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1522,7 +1471,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Sheet1 (2)'!$K$3:$L$13</c:f>
+              <c:f>Sheet1!$K$3:$L$13</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="11"/>
                 <c:lvl>
@@ -1600,36 +1549,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet1 (2)'!$N$3:$N$13</c:f>
+              <c:f>Sheet1!$N$3:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.13207547169811321</c:v>
+                  <c:v>0.16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.5471698113207544E-2</c:v>
+                  <c:v>0.32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11320754716981132</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11320754716981132</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11320754716981132</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.11320754716981132</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.11320754716981132</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.11320754716981132</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.11320754716981132</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -1642,7 +1591,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-6130-4703-A271-EBB8FC5EFE15}"/>
+              <c16:uniqueId val="{00000001-8306-4031-ABC8-1844283DA1A9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1656,11 +1605,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="559623792"/>
-        <c:axId val="559624120"/>
+        <c:axId val="769597072"/>
+        <c:axId val="769597728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="559623792"/>
+        <c:axId val="769597072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1703,7 +1652,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="559624120"/>
+        <c:crossAx val="769597728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1711,7 +1660,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="559624120"/>
+        <c:axId val="769597728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1762,7 +1711,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="559623792"/>
+        <c:crossAx val="769597072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1905,7 +1854,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sheet1 (3)'!$M$2</c:f>
+              <c:f>'Sheet1 (2)'!$M$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1926,7 +1875,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Sheet1 (3)'!$K$3:$L$13</c:f>
+              <c:f>'Sheet1 (2)'!$K$3:$L$13</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="11"/>
                 <c:lvl>
@@ -2004,46 +1953,43 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet1 (3)'!$M$3:$M$13</c:f>
+              <c:f>'Sheet1 (2)'!$M$3:$M$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8CD8-4586-8FD7-0BD079CE6269}"/>
+              <c16:uniqueId val="{00000000-FEEE-481E-9A6E-45F4A636FEF0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2052,7 +1998,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sheet1 (3)'!$N$2</c:f>
+              <c:f>'Sheet1 (2)'!$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2073,7 +2019,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Sheet1 (3)'!$K$3:$L$13</c:f>
+              <c:f>'Sheet1 (2)'!$K$3:$L$13</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="11"/>
                 <c:lvl>
@@ -2151,39 +2097,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet1 (3)'!$N$3:$N$13</c:f>
+              <c:f>'Sheet1 (2)'!$N$3:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>7.6086956521739135E-2</c:v>
+                  <c:v>0.1038961038961039</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.6086956521739135E-2</c:v>
+                  <c:v>7.792207792207792E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.6086956521739135E-2</c:v>
+                  <c:v>0.11688311688311688</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.6086956521739135E-2</c:v>
+                  <c:v>0.11688311688311688</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.31521739130434784</c:v>
+                  <c:v>0.11688311688311688</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.6086956521739135E-2</c:v>
+                  <c:v>0.11688311688311688</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.6086956521739135E-2</c:v>
+                  <c:v>0.11688311688311688</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.6086956521739135E-2</c:v>
+                  <c:v>0.11688311688311688</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.6086956521739135E-2</c:v>
+                  <c:v>0.11688311688311688</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.6086956521739135E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -2193,7 +2139,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8CD8-4586-8FD7-0BD079CE6269}"/>
+              <c16:uniqueId val="{00000001-FEEE-481E-9A6E-45F4A636FEF0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2207,11 +2153,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="562510384"/>
-        <c:axId val="562510712"/>
+        <c:axId val="556936144"/>
+        <c:axId val="544536952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="562510384"/>
+        <c:axId val="556936144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2254,7 +2200,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="562510712"/>
+        <c:crossAx val="544536952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2262,7 +2208,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="562510712"/>
+        <c:axId val="544536952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2313,7 +2259,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="562510384"/>
+        <c:crossAx val="556936144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2456,7 +2402,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sheet1 (4)'!$M$2</c:f>
+              <c:f>'Sheet1 (3)'!$M$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2477,7 +2423,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Sheet1 (4)'!$K$3:$L$13</c:f>
+              <c:f>'Sheet1 (3)'!$K$3:$L$13</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="11"/>
                 <c:lvl>
@@ -2555,46 +2501,46 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet1 (4)'!$M$3:$M$13</c:f>
+              <c:f>'Sheet1 (3)'!$M$3:$M$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6E4B-47A8-AE4A-F723D1391D3E}"/>
+              <c16:uniqueId val="{00000000-EDB8-4961-9F75-43B96E13F76D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2603,7 +2549,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sheet1 (4)'!$N$2</c:f>
+              <c:f>'Sheet1 (3)'!$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2624,7 +2570,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Sheet1 (4)'!$K$3:$L$13</c:f>
+              <c:f>'Sheet1 (3)'!$K$3:$L$13</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="11"/>
                 <c:lvl>
@@ -2702,39 +2648,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet1 (4)'!$N$3:$N$13</c:f>
+              <c:f>'Sheet1 (3)'!$N$3:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.13559322033898305</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.4745762711864403E-2</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.4745762711864403E-2</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1864406779661017</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.4745762711864403E-2</c:v>
+                  <c:v>0.28000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.4745762711864403E-2</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.4745762711864403E-2</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.4745762711864403E-2</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.4745762711864403E-2</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.4745762711864403E-2</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -2744,7 +2690,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-6E4B-47A8-AE4A-F723D1391D3E}"/>
+              <c16:uniqueId val="{00000001-EDB8-4961-9F75-43B96E13F76D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2758,11 +2704,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="383303584"/>
-        <c:axId val="383299648"/>
+        <c:axId val="556416608"/>
+        <c:axId val="556419888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="383303584"/>
+        <c:axId val="556416608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2805,7 +2751,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="383299648"/>
+        <c:crossAx val="556419888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2813,7 +2759,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="383299648"/>
+        <c:axId val="556419888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2864,7 +2810,558 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="383303584"/>
+        <c:crossAx val="556416608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet1 (4)'!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Sheet1 (4)'!$K$3:$L$13</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="11"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Student did not download Exam</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Monitor file not uploaded</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Student did not upload exam file</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Student received second download</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Student was not able to complete exam</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Student verifcation failed</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>test code</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>test code 8</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>test code 9</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>testcode 10</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>code 11</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>7</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>8</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>9</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>11</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (4)'!$M$3:$M$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C988-4414-8C6A-29F60043553B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet1 (4)'!$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>% of Total Errors</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Sheet1 (4)'!$K$3:$L$13</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="11"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Student did not download Exam</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Monitor file not uploaded</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Student did not upload exam file</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Student received second download</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Student was not able to complete exam</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Student verifcation failed</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>test code</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>test code 8</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>test code 9</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>testcode 10</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>code 11</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>7</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>8</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>9</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>11</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (4)'!$N$3:$N$13</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.14285714285714285</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.5714285714285715E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.5714285714285715E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17142857142857143</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.5714285714285715E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.5714285714285715E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.5714285714285715E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.5714285714285715E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.5714285714285715E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.5714285714285715E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C988-4414-8C6A-29F60043553B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="556412016"/>
+        <c:axId val="556413984"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="556412016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="556413984"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="556413984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="556412016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3111,6 +3608,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -5123,27 +5660,530 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1747837</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>6</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>6</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2357437</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>476250</xdr:rowOff>
+      <xdr:colOff>304806</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76206</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE023DE3-A7D4-4774-8DCA-DB42623D2A6D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07D0B528-42FF-4960-9D62-D85637C30C8D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5168,23 +6208,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1747837</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>6</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>6</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>2357437</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>476250</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1200156</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>304806</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C9A5F7B-1DB4-4250-BFB7-DA9E3404AE24}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8350B8E4-F94D-41B7-B3D6-07D82B97180E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5209,23 +6249,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1262062</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>6</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>6</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>509587</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>490537</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1200156</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>304806</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE811510-994B-4177-9183-5DC34A9CF71C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2717283-7510-4374-BAD5-4E03F3C6B870}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5250,23 +6290,64 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>3000375</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>6</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>6</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>781050</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>457200</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>733431</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>304806</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4068787-9786-4696-BB69-E9B9EEFC2EA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEA958ED-ED65-4B29-8DE5-C33771B3EFE6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>6</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>6</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2466981</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>304806</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29B32CDC-1C60-4A60-B318-18B113BDB13E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5288,16 +6369,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{66EBEDC1-001E-4FA9-B050-8F29302F975C}" name="ErrorCode" displayName="ErrorCode" ref="K2:N14" totalsRowCount="1">
-  <autoFilter ref="K2:N13" xr:uid="{7827120D-4936-4D2F-9092-54419C75C585}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{510344EE-EBDA-403D-8040-97C20E5CE921}" name="ErrorCode6" displayName="ErrorCode6" ref="K2:N14" totalsRowCount="1">
+  <autoFilter ref="K2:N13" xr:uid="{03B136F6-5AC7-4BDD-8572-02A2CD6E7F1B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F9ADB14C-6A92-4202-B545-6B3F3C19A244}" name="Error code"/>
-    <tableColumn id="2" xr3:uid="{DCF61CD2-3D93-4107-80DB-40E7900BB5D9}" name="Description"/>
-    <tableColumn id="3" xr3:uid="{9343BE5D-CF05-43CB-814E-30BDFDA4D28E}" name="Total" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(ErrorCode[Total])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{1A5A4717-CBED-4F39-82DF-4CE99E0BD5F6}" name="% of Total Errors" totalsRowFunction="average" totalsRowDxfId="3" dataCellStyle="Percent">
-      <calculatedColumnFormula>ErrorCode[[#This Row],[Total]]/ErrorCode[[#Totals],[Total]]</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{361A701B-D61A-4935-B652-608BC3CA7B25}" name="Error code"/>
+    <tableColumn id="2" xr3:uid="{DBC67356-1CF5-4762-918A-047A092A0D5A}" name="Description"/>
+    <tableColumn id="3" xr3:uid="{FA1639E0-DFD9-41B9-81EE-45C21E3F4AE8}" name="Total" totalsRowLabel="188"/>
+    <tableColumn id="4" xr3:uid="{C742CF39-09B9-4BEC-843C-4D12685BFA12}" name="% of Total Errors" totalsRowFunction="custom" totalsRowDxfId="0" dataCellStyle="Percent">
+      <calculatedColumnFormula>ErrorCode6[[#This Row],[Total]]/ErrorCode6[[#Totals],[Total]]</calculatedColumnFormula>
+      <totalsRowFormula>SUM(ErrorCode6[% of Total Errors])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5305,16 +6385,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1968EC46-FBCA-4DA1-8119-8F6CB029D49E}" name="ErrorCode3" displayName="ErrorCode3" ref="K2:N14" totalsRowCount="1">
-  <autoFilter ref="K2:N13" xr:uid="{E8A270FF-2DC9-40A6-A14E-14133A86883B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{516F4C30-2DA1-4DA6-8ED7-53B2FEBFA0F5}" name="ErrorCode" displayName="ErrorCode" ref="K2:N14" totalsRowCount="1">
+  <autoFilter ref="K2:N13" xr:uid="{9C8B4A28-3175-4666-8A07-77699E6E3A76}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C12C0C52-94FF-49EB-87B4-3FCDBAF7359A}" name="Error code"/>
-    <tableColumn id="2" xr3:uid="{395174B4-DF0A-486F-A0AC-AD3B5C686DA2}" name="Description"/>
-    <tableColumn id="3" xr3:uid="{A0323B96-1483-4E45-9A2F-3267CDA75759}" name="Total" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(ErrorCode3[Total])</totalsRowFormula>
+    <tableColumn id="1" xr3:uid="{60DC970A-DF1A-4D11-9CFD-AFF028834997}" name="Error code"/>
+    <tableColumn id="2" xr3:uid="{F80C0F03-B053-4BD1-8356-F959768D3C2E}" name="Description"/>
+    <tableColumn id="3" xr3:uid="{B2FE9862-4134-4246-92B5-0E7BB284FC33}" name="Total" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(ErrorCode[Total])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DA6FD53C-30E0-420E-B407-DA41BF638BCD}" name="% of Total Errors" totalsRowFunction="average" totalsRowDxfId="2" dataCellStyle="Percent">
-      <calculatedColumnFormula>ErrorCode3[[#This Row],[Total]]/ErrorCode3[[#Totals],[Total]]</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{F4E26A16-A463-41EF-899A-5B2C7D59422C}" name="% of Total Errors" totalsRowFunction="custom" totalsRowDxfId="4" dataCellStyle="Percent">
+      <calculatedColumnFormula>ErrorCode[[#This Row],[Total]]/ErrorCode[[#Totals],[Total]]</calculatedColumnFormula>
+      <totalsRowFormula>SUM(ErrorCode[% of Total Errors])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5322,16 +6403,17 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{22D94AA4-3C1B-450A-B905-64D91B3E2C92}" name="ErrorCode4" displayName="ErrorCode4" ref="K2:N14" totalsRowCount="1">
-  <autoFilter ref="K2:N13" xr:uid="{19F73FFB-8E7D-498B-BC79-29771FD4D75E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BF14FCA6-6F56-4A18-AC11-8731396B3429}" name="ErrorCode3" displayName="ErrorCode3" ref="K2:N14" totalsRowCount="1">
+  <autoFilter ref="K2:N13" xr:uid="{2862DF6F-A3DF-4A95-8182-861E6D796083}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3C63CA1B-C75A-4E2B-A0CF-45C0DDD1D038}" name="Error code"/>
-    <tableColumn id="2" xr3:uid="{7B35371C-E06D-4E92-929C-66EE69D3BEE2}" name="Description"/>
-    <tableColumn id="3" xr3:uid="{A39F19A2-6EAF-4F22-B16C-F1FC3D7D27F0}" name="Total" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(ErrorCode4[Total])</totalsRowFormula>
+    <tableColumn id="1" xr3:uid="{F4ED194D-9A87-474F-BCB1-142BE90010A9}" name="Error code"/>
+    <tableColumn id="2" xr3:uid="{E491639B-C5F9-4115-A9D4-1A355BBDD2BC}" name="Description"/>
+    <tableColumn id="3" xr3:uid="{C756F23C-6634-4DE7-9079-A52D02651A90}" name="Total" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(ErrorCode3[Total])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C940FE58-37F8-4975-AC59-5B2BCC8640D4}" name="% of Total Errors" totalsRowFunction="average" totalsRowDxfId="1" dataCellStyle="Percent">
-      <calculatedColumnFormula>ErrorCode4[[#This Row],[Total]]/ErrorCode4[[#Totals],[Total]]</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{8B438750-E968-464C-A29C-DC1A57F22813}" name="% of Total Errors" totalsRowFunction="custom" totalsRowDxfId="3" dataCellStyle="Percent">
+      <calculatedColumnFormula>ErrorCode3[[#This Row],[Total]]/ErrorCode3[[#Totals],[Total]]</calculatedColumnFormula>
+      <totalsRowFormula>SUM(ErrorCode3[% of Total Errors])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5339,16 +6421,35 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{55F84671-0D97-4C99-8F46-4D357B2AE56D}" name="ErrorCode5" displayName="ErrorCode5" ref="K2:N14" totalsRowCount="1">
-  <autoFilter ref="K2:N13" xr:uid="{64C37D6D-5443-4983-9454-10C301BB4702}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9B112D0A-B8FE-4BF5-A3BC-65049F6A1EEF}" name="ErrorCode4" displayName="ErrorCode4" ref="K2:N14" totalsRowCount="1">
+  <autoFilter ref="K2:N13" xr:uid="{8AFCAEC6-C56B-499E-BFF2-8D2840591799}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{038B1E29-4B9F-4FCD-82B7-28DCE21889B5}" name="Error code"/>
-    <tableColumn id="2" xr3:uid="{91F2B7F8-9C9E-4A2E-8EA9-8B7F79CD5DBA}" name="Description"/>
-    <tableColumn id="3" xr3:uid="{CF0B141E-A4A3-49F2-BB4F-B32F3433EEA6}" name="Total" totalsRowFunction="custom">
+    <tableColumn id="1" xr3:uid="{86BAC067-8F9C-4B7C-A43E-35FCF806F734}" name="Error code"/>
+    <tableColumn id="2" xr3:uid="{196E0CBA-8E59-4D26-BCB2-6C16074DE939}" name="Description"/>
+    <tableColumn id="3" xr3:uid="{796E7CD1-22B2-42D7-8A87-CFDB0CBA3DD4}" name="Total" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(ErrorCode4[Total])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{859855CF-6180-4FB9-9D30-832EE5B28174}" name="% of Total Errors" totalsRowFunction="custom" totalsRowDxfId="2" dataCellStyle="Percent">
+      <calculatedColumnFormula>ErrorCode4[[#This Row],[Total]]/ErrorCode4[[#Totals],[Total]]</calculatedColumnFormula>
+      <totalsRowFormula>SUM(ErrorCode4[% of Total Errors])</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D6152E39-6198-44DC-8D1A-D01941A57C34}" name="ErrorCode5" displayName="ErrorCode5" ref="K2:N14" totalsRowCount="1">
+  <autoFilter ref="K2:N13" xr:uid="{3149404B-0B3F-4766-8F53-0FC923987C66}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{2639FB75-E48A-46B3-BC6B-0A295BD330D1}" name="Error code"/>
+    <tableColumn id="2" xr3:uid="{8B82E086-BA01-46BB-8361-050EE2D8B6C3}" name="Description"/>
+    <tableColumn id="3" xr3:uid="{B7C8FFB0-E45F-44AD-BD54-FEDAE1424E50}" name="Total" totalsRowFunction="custom">
       <totalsRowFormula>SUM(ErrorCode5[Total])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{134390AA-AC28-4803-88D7-F8C0B1899AD8}" name="% of Total Errors" totalsRowFunction="average" totalsRowDxfId="0" dataCellStyle="Percent">
+    <tableColumn id="4" xr3:uid="{6ACEB675-D078-4BB3-BC72-EA1D4BBE8F8F}" name="% of Total Errors" totalsRowFunction="custom" totalsRowDxfId="1" dataCellStyle="Percent">
       <calculatedColumnFormula>ErrorCode5[[#This Row],[Total]]/ErrorCode5[[#Totals],[Total]]</calculatedColumnFormula>
+      <totalsRowFormula>SUM(ErrorCode5[% of Total Errors])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5651,6 +6752,211 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500D4B20-C4CB-4368-B69B-968BC3A919A7}">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="K2:N14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:N14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M2" t="s">
+        <v>73</v>
+      </c>
+      <c r="N2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>74</v>
+      </c>
+      <c r="M3">
+        <v>21</v>
+      </c>
+      <c r="N3" s="42">
+        <f>ErrorCode6[[#This Row],[Total]]/ErrorCode6[[#Totals],[Total]]</f>
+        <v>0.11170212765957446</v>
+      </c>
+    </row>
+    <row r="4" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>75</v>
+      </c>
+      <c r="M4">
+        <v>21</v>
+      </c>
+      <c r="N4" s="42">
+        <f>ErrorCode6[[#This Row],[Total]]/ErrorCode6[[#Totals],[Total]]</f>
+        <v>0.11170212765957446</v>
+      </c>
+    </row>
+    <row r="5" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M5">
+        <v>22</v>
+      </c>
+      <c r="N5" s="42">
+        <f>ErrorCode6[[#This Row],[Total]]/ErrorCode6[[#Totals],[Total]]</f>
+        <v>0.11702127659574468</v>
+      </c>
+    </row>
+    <row r="6" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6" t="s">
+        <v>77</v>
+      </c>
+      <c r="M6">
+        <v>22</v>
+      </c>
+      <c r="N6" s="42">
+        <f>ErrorCode6[[#This Row],[Total]]/ErrorCode6[[#Totals],[Total]]</f>
+        <v>0.11702127659574468</v>
+      </c>
+    </row>
+    <row r="7" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="L7" t="s">
+        <v>78</v>
+      </c>
+      <c r="M7">
+        <v>29</v>
+      </c>
+      <c r="N7" s="42">
+        <f>ErrorCode6[[#This Row],[Total]]/ErrorCode6[[#Totals],[Total]]</f>
+        <v>0.15425531914893617</v>
+      </c>
+    </row>
+    <row r="8" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>6</v>
+      </c>
+      <c r="L8" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="M8">
+        <v>17</v>
+      </c>
+      <c r="N8" s="42">
+        <f>ErrorCode6[[#This Row],[Total]]/ErrorCode6[[#Totals],[Total]]</f>
+        <v>9.0425531914893623E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>7</v>
+      </c>
+      <c r="L9" t="s">
+        <v>80</v>
+      </c>
+      <c r="M9">
+        <v>16</v>
+      </c>
+      <c r="N9" s="42">
+        <f>ErrorCode6[[#This Row],[Total]]/ErrorCode6[[#Totals],[Total]]</f>
+        <v>8.5106382978723402E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>8</v>
+      </c>
+      <c r="L10" t="s">
+        <v>81</v>
+      </c>
+      <c r="M10">
+        <v>16</v>
+      </c>
+      <c r="N10" s="42">
+        <f>ErrorCode6[[#This Row],[Total]]/ErrorCode6[[#Totals],[Total]]</f>
+        <v>8.5106382978723402E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>9</v>
+      </c>
+      <c r="L11" t="s">
+        <v>82</v>
+      </c>
+      <c r="M11">
+        <v>16</v>
+      </c>
+      <c r="N11" s="42">
+        <f>ErrorCode6[[#This Row],[Total]]/ErrorCode6[[#Totals],[Total]]</f>
+        <v>8.5106382978723402E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>10</v>
+      </c>
+      <c r="L12" t="s">
+        <v>83</v>
+      </c>
+      <c r="M12">
+        <v>7</v>
+      </c>
+      <c r="N12" s="42">
+        <f>ErrorCode6[[#This Row],[Total]]/ErrorCode6[[#Totals],[Total]]</f>
+        <v>3.7234042553191488E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>11</v>
+      </c>
+      <c r="L13" t="s">
+        <v>89</v>
+      </c>
+      <c r="N13" s="42">
+        <f>ErrorCode6[[#This Row],[Total]]/ErrorCode6[[#Totals],[Total]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="M14" t="s">
+        <v>91</v>
+      </c>
+      <c r="N14" s="43">
+        <f>SUM(ErrorCode6[% of Total Errors])</f>
+        <v>0.99468085106382986</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{570E0E29-0EF2-46E6-BDFB-1E1208C600DE}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N133"/>
@@ -5735,7 +7041,7 @@
         <v>74</v>
       </c>
       <c r="M3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N3" s="42">
         <f>ErrorCode[[#This Row],[Total]]/ErrorCode[[#Totals],[Total]]</f>
@@ -5772,7 +7078,7 @@
         <v>75</v>
       </c>
       <c r="M4">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="N4" s="42">
         <f>ErrorCode[[#This Row],[Total]]/ErrorCode[[#Totals],[Total]]</f>
@@ -5809,7 +7115,7 @@
         <v>76</v>
       </c>
       <c r="M5">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="N5" s="42">
         <f>ErrorCode[[#This Row],[Total]]/ErrorCode[[#Totals],[Total]]</f>
@@ -5846,7 +7152,7 @@
         <v>77</v>
       </c>
       <c r="M6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="N6" s="42">
         <f>ErrorCode[[#This Row],[Total]]/ErrorCode[[#Totals],[Total]]</f>
@@ -5883,7 +7189,7 @@
         <v>78</v>
       </c>
       <c r="M7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="N7" s="42">
         <f>ErrorCode[[#This Row],[Total]]/ErrorCode[[#Totals],[Total]]</f>
@@ -5920,7 +7226,7 @@
         <v>79</v>
       </c>
       <c r="M8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N8" s="42">
         <f>ErrorCode[[#This Row],[Total]]/ErrorCode[[#Totals],[Total]]</f>
@@ -6111,11 +7417,11 @@
       <c r="L14"/>
       <c r="M14">
         <f>SUM(ErrorCode[Total])</f>
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="N14" s="43">
-        <f>SUBTOTAL(101,ErrorCode[% of Total Errors])</f>
-        <v>9.0909090909090912E-2</v>
+        <f>SUM(ErrorCode[% of Total Errors])</f>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -7390,7 +8696,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00B18458-A220-48F1-9A3B-F334B60942DD}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N133"/>
@@ -7475,11 +8781,11 @@
         <v>74</v>
       </c>
       <c r="M3">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="N3" s="42">
         <f>ErrorCode3[[#This Row],[Total]]/ErrorCode3[[#Totals],[Total]]</f>
-        <v>0.13207547169811321</v>
+        <v>0.1038961038961039</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -7512,11 +8818,11 @@
         <v>75</v>
       </c>
       <c r="M4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N4" s="42">
         <f>ErrorCode3[[#This Row],[Total]]/ErrorCode3[[#Totals],[Total]]</f>
-        <v>7.5471698113207544E-2</v>
+        <v>7.792207792207792E-2</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -7549,11 +8855,11 @@
         <v>76</v>
       </c>
       <c r="M5">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="N5" s="42">
         <f>ErrorCode3[[#This Row],[Total]]/ErrorCode3[[#Totals],[Total]]</f>
-        <v>0.11320754716981132</v>
+        <v>0.11688311688311688</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -7586,11 +8892,11 @@
         <v>77</v>
       </c>
       <c r="M6">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="N6" s="42">
         <f>ErrorCode3[[#This Row],[Total]]/ErrorCode3[[#Totals],[Total]]</f>
-        <v>0.11320754716981132</v>
+        <v>0.11688311688311688</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -7623,11 +8929,11 @@
         <v>78</v>
       </c>
       <c r="M7">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="N7" s="42">
         <f>ErrorCode3[[#This Row],[Total]]/ErrorCode3[[#Totals],[Total]]</f>
-        <v>0.11320754716981132</v>
+        <v>0.11688311688311688</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -7660,11 +8966,11 @@
         <v>79</v>
       </c>
       <c r="M8">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="N8" s="42">
         <f>ErrorCode3[[#This Row],[Total]]/ErrorCode3[[#Totals],[Total]]</f>
-        <v>0.11320754716981132</v>
+        <v>0.11688311688311688</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -7697,11 +9003,11 @@
         <v>80</v>
       </c>
       <c r="M9">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="N9" s="42">
         <f>ErrorCode3[[#This Row],[Total]]/ErrorCode3[[#Totals],[Total]]</f>
-        <v>0.11320754716981132</v>
+        <v>0.11688311688311688</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -7734,11 +9040,11 @@
         <v>81</v>
       </c>
       <c r="M10">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="N10" s="42">
         <f>ErrorCode3[[#This Row],[Total]]/ErrorCode3[[#Totals],[Total]]</f>
-        <v>0.11320754716981132</v>
+        <v>0.11688311688311688</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -7771,11 +9077,11 @@
         <v>82</v>
       </c>
       <c r="M11">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="N11" s="42">
         <f>ErrorCode3[[#This Row],[Total]]/ErrorCode3[[#Totals],[Total]]</f>
-        <v>0.11320754716981132</v>
+        <v>0.11688311688311688</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -7861,11 +9167,11 @@
       <c r="L14"/>
       <c r="M14">
         <f>SUM(ErrorCode3[Total])</f>
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="N14" s="43">
-        <f>SUBTOTAL(101,ErrorCode3[% of Total Errors])</f>
-        <v>9.0909090909090898E-2</v>
+        <f>SUM(ErrorCode3[% of Total Errors])</f>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -9116,7 +10422,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15BF9FC7-5283-4008-A427-53C947F9BFDD}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:N133"/>
@@ -9201,11 +10507,11 @@
         <v>74</v>
       </c>
       <c r="M3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="N3" s="42">
         <f>ErrorCode4[[#This Row],[Total]]/ErrorCode4[[#Totals],[Total]]</f>
-        <v>7.6086956521739135E-2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -9238,11 +10544,11 @@
         <v>75</v>
       </c>
       <c r="M4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="N4" s="42">
         <f>ErrorCode4[[#This Row],[Total]]/ErrorCode4[[#Totals],[Total]]</f>
-        <v>7.6086956521739135E-2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -9275,11 +10581,11 @@
         <v>76</v>
       </c>
       <c r="M5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="N5" s="42">
         <f>ErrorCode4[[#This Row],[Total]]/ErrorCode4[[#Totals],[Total]]</f>
-        <v>7.6086956521739135E-2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -9312,11 +10618,11 @@
         <v>77</v>
       </c>
       <c r="M6">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="N6" s="42">
         <f>ErrorCode4[[#This Row],[Total]]/ErrorCode4[[#Totals],[Total]]</f>
-        <v>7.6086956521739135E-2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -9349,11 +10655,11 @@
         <v>78</v>
       </c>
       <c r="M7">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="N7" s="42">
         <f>ErrorCode4[[#This Row],[Total]]/ErrorCode4[[#Totals],[Total]]</f>
-        <v>0.31521739130434784</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -9386,11 +10692,11 @@
         <v>79</v>
       </c>
       <c r="M8">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="N8" s="42">
         <f>ErrorCode4[[#This Row],[Total]]/ErrorCode4[[#Totals],[Total]]</f>
-        <v>7.6086956521739135E-2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -9423,11 +10729,11 @@
         <v>80</v>
       </c>
       <c r="M9">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="N9" s="42">
         <f>ErrorCode4[[#This Row],[Total]]/ErrorCode4[[#Totals],[Total]]</f>
-        <v>7.6086956521739135E-2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -9460,11 +10766,11 @@
         <v>81</v>
       </c>
       <c r="M10">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="N10" s="42">
         <f>ErrorCode4[[#This Row],[Total]]/ErrorCode4[[#Totals],[Total]]</f>
-        <v>7.6086956521739135E-2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -9497,11 +10803,11 @@
         <v>82</v>
       </c>
       <c r="M11">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="N11" s="42">
         <f>ErrorCode4[[#This Row],[Total]]/ErrorCode4[[#Totals],[Total]]</f>
-        <v>7.6086956521739135E-2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -9522,11 +10828,11 @@
         <v>83</v>
       </c>
       <c r="M12">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="N12" s="42">
         <f>ErrorCode4[[#This Row],[Total]]/ErrorCode4[[#Totals],[Total]]</f>
-        <v>7.6086956521739135E-2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -9583,11 +10889,11 @@
       <c r="L14"/>
       <c r="M14">
         <f>SUM(ErrorCode4[Total])</f>
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="N14" s="43">
-        <f>SUBTOTAL(101,ErrorCode4[% of Total Errors])</f>
-        <v>9.0909090909090912E-2</v>
+        <f>SUM(ErrorCode4[% of Total Errors])</f>
+        <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -10872,12 +12178,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252E5F95-DB34-4330-9091-F42B49558D5E}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:N133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K2" sqref="K2:N14"/>
     </sheetView>
   </sheetViews>
@@ -10957,11 +12263,11 @@
         <v>74</v>
       </c>
       <c r="M3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N3" s="42">
         <f>ErrorCode5[[#This Row],[Total]]/ErrorCode5[[#Totals],[Total]]</f>
-        <v>0.13559322033898305</v>
+        <v>0.14285714285714285</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -10994,11 +12300,11 @@
         <v>75</v>
       </c>
       <c r="M4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N4" s="42">
         <f>ErrorCode5[[#This Row],[Total]]/ErrorCode5[[#Totals],[Total]]</f>
-        <v>8.4745762711864403E-2</v>
+        <v>8.5714285714285715E-2</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -11031,11 +12337,11 @@
         <v>76</v>
       </c>
       <c r="M5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N5" s="42">
         <f>ErrorCode5[[#This Row],[Total]]/ErrorCode5[[#Totals],[Total]]</f>
-        <v>8.4745762711864403E-2</v>
+        <v>8.5714285714285715E-2</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -11068,11 +12374,11 @@
         <v>77</v>
       </c>
       <c r="M6">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="N6" s="42">
         <f>ErrorCode5[[#This Row],[Total]]/ErrorCode5[[#Totals],[Total]]</f>
-        <v>0.1864406779661017</v>
+        <v>0.17142857142857143</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -11105,11 +12411,11 @@
         <v>78</v>
       </c>
       <c r="M7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N7" s="42">
         <f>ErrorCode5[[#This Row],[Total]]/ErrorCode5[[#Totals],[Total]]</f>
-        <v>8.4745762711864403E-2</v>
+        <v>8.5714285714285715E-2</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -11142,11 +12448,11 @@
         <v>79</v>
       </c>
       <c r="M8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N8" s="42">
         <f>ErrorCode5[[#This Row],[Total]]/ErrorCode5[[#Totals],[Total]]</f>
-        <v>8.4745762711864403E-2</v>
+        <v>8.5714285714285715E-2</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -11179,11 +12485,11 @@
         <v>80</v>
       </c>
       <c r="M9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N9" s="42">
         <f>ErrorCode5[[#This Row],[Total]]/ErrorCode5[[#Totals],[Total]]</f>
-        <v>8.4745762711864403E-2</v>
+        <v>8.5714285714285715E-2</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -11216,11 +12522,11 @@
         <v>81</v>
       </c>
       <c r="M10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N10" s="42">
         <f>ErrorCode5[[#This Row],[Total]]/ErrorCode5[[#Totals],[Total]]</f>
-        <v>8.4745762711864403E-2</v>
+        <v>8.5714285714285715E-2</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -11253,11 +12559,11 @@
         <v>82</v>
       </c>
       <c r="M11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N11" s="42">
         <f>ErrorCode5[[#This Row],[Total]]/ErrorCode5[[#Totals],[Total]]</f>
-        <v>8.4745762711864403E-2</v>
+        <v>8.5714285714285715E-2</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -11276,11 +12582,11 @@
         <v>83</v>
       </c>
       <c r="M12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N12" s="42">
         <f>ErrorCode5[[#This Row],[Total]]/ErrorCode5[[#Totals],[Total]]</f>
-        <v>8.4745762711864403E-2</v>
+        <v>8.5714285714285715E-2</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -11331,11 +12637,11 @@
       <c r="L14"/>
       <c r="M14">
         <f>SUM(ErrorCode5[Total])</f>
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="N14" s="43">
-        <f>SUBTOTAL(101,ErrorCode5[% of Total Errors])</f>
-        <v>9.0909090909090912E-2</v>
+        <f>SUM(ErrorCode5[% of Total Errors])</f>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added code for collecting raw totals data from each worksheet table and then compiling that data into a table on the final runningReport tab. A scatter plot was selected as the metodof displaying that data.
</commit_message>
<xml_diff>
--- a/VisualizeTest.xlsx
+++ b/VisualizeTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\VBA\ReportVisualization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80191C9D-59E9-4A1B-84FC-0370A530242D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83879926-3408-4C08-8CD7-12954F8318EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1950" yWindow="1200" windowWidth="8415" windowHeight="12345" activeTab="4" xr2:uid="{34CDE331-2BE0-4989-A0C3-15C3DC22DD25}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{34CDE331-2BE0-4989-A0C3-15C3DC22DD25}"/>
   </bookViews>
   <sheets>
     <sheet name="RunningReport" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="96">
   <si>
     <t>PCM2 EXAM4 (BSCE BK3) - PART 1-3</t>
   </si>
@@ -341,6 +341,18 @@
   </si>
   <si>
     <t>188</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
+  </si>
+  <si>
+    <t>Sheet1 (2)</t>
+  </si>
+  <si>
+    <t>Sheet1 (3)</t>
+  </si>
+  <si>
+    <t>Sheet1 (4)</t>
   </si>
 </sst>
 </file>
@@ -785,7 +797,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.2692038495188102E-2"/>
+          <c:y val="7.407407407407407E-2"/>
+          <c:w val="0.90286351706036749"/>
+          <c:h val="0.37334718576844561"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -933,7 +955,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2D26-43DB-AE58-6145CBCEC192}"/>
+              <c16:uniqueId val="{00000000-94AB-4B7C-BA6A-3D86FA0CB074}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1083,7 +1105,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2D26-43DB-AE58-6145CBCEC192}"/>
+              <c16:uniqueId val="{00000001-94AB-4B7C-BA6A-3D86FA0CB074}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1097,11 +1119,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="568689104"/>
-        <c:axId val="568689432"/>
+        <c:axId val="539556024"/>
+        <c:axId val="551430632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="568689104"/>
+        <c:axId val="539556024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1144,7 +1166,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="568689432"/>
+        <c:crossAx val="551430632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1152,7 +1174,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="568689432"/>
+        <c:axId val="551430632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1203,7 +1225,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="568689104"/>
+        <c:crossAx val="539556024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1441,7 +1463,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8C01-403B-B20E-E5AB1D8AFA4E}"/>
+              <c16:uniqueId val="{00000000-E612-479F-878F-D5B7C2DA88BE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1591,7 +1613,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8C01-403B-B20E-E5AB1D8AFA4E}"/>
+              <c16:uniqueId val="{00000001-E612-479F-878F-D5B7C2DA88BE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1605,11 +1627,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="571889392"/>
-        <c:axId val="571889064"/>
+        <c:axId val="541932056"/>
+        <c:axId val="541934024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="571889392"/>
+        <c:axId val="541932056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1652,7 +1674,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="571889064"/>
+        <c:crossAx val="541934024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1660,7 +1682,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="571889064"/>
+        <c:axId val="541934024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1711,7 +1733,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="571889392"/>
+        <c:crossAx val="541932056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1989,7 +2011,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E7D2-4B11-A480-F0DAABB5229F}"/>
+              <c16:uniqueId val="{00000000-71A7-415D-A303-8559F0240AD1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2139,7 +2161,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E7D2-4B11-A480-F0DAABB5229F}"/>
+              <c16:uniqueId val="{00000001-71A7-415D-A303-8559F0240AD1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2153,11 +2175,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="573366152"/>
-        <c:axId val="573366808"/>
+        <c:axId val="541919264"/>
+        <c:axId val="541914016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="573366152"/>
+        <c:axId val="541919264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2200,7 +2222,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="573366808"/>
+        <c:crossAx val="541914016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2208,7 +2230,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="573366808"/>
+        <c:axId val="541914016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2259,7 +2281,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="573366152"/>
+        <c:crossAx val="541919264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2540,7 +2562,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-34DE-48F9-9EBC-5DD466CD5DD3}"/>
+              <c16:uniqueId val="{00000000-3C73-4C88-AA4E-7B4834DDCBB4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2690,7 +2712,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-34DE-48F9-9EBC-5DD466CD5DD3}"/>
+              <c16:uniqueId val="{00000001-3C73-4C88-AA4E-7B4834DDCBB4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2704,11 +2726,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="572067016"/>
-        <c:axId val="572065048"/>
+        <c:axId val="544677536"/>
+        <c:axId val="544678192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="572067016"/>
+        <c:axId val="544677536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2751,7 +2773,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="572065048"/>
+        <c:crossAx val="544678192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2759,7 +2781,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="572065048"/>
+        <c:axId val="544678192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2810,7 +2832,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="572067016"/>
+        <c:crossAx val="544677536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3091,7 +3113,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5F79-4222-B201-EF16935AACB1}"/>
+              <c16:uniqueId val="{00000000-AAD5-456F-8186-F4D72C49EA74}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3241,7 +3263,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5F79-4222-B201-EF16935AACB1}"/>
+              <c16:uniqueId val="{00000001-AAD5-456F-8186-F4D72C49EA74}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3255,11 +3277,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="568686808"/>
-        <c:axId val="568683528"/>
+        <c:axId val="374620896"/>
+        <c:axId val="374623520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="568686808"/>
+        <c:axId val="374620896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3302,7 +3324,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="568683528"/>
+        <c:crossAx val="374623520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3310,7 +3332,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="568683528"/>
+        <c:axId val="374623520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3361,7 +3383,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="568686808"/>
+        <c:crossAx val="374620896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6167,23 +6189,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B0BF35A-258B-4D25-B60F-BE16BEC5992E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{710DA091-D319-4074-B532-3159B02D99EA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6221,10 +6243,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C2EA416-C134-4C7A-8ED7-AB1DB2527368}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6593BD3A-6221-452E-AB3B-8F08C2F753D4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6262,10 +6284,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F980EE1-21B5-4A3B-9B02-9BD1764BBBCD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75E98E6D-9BD0-43A5-A299-67BDCE6833FE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6303,10 +6325,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE424136-7D9E-4B4E-8420-8D5499CFAB94}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1ECB0563-A22C-4B96-9D20-55AC30F620FC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6344,10 +6366,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7567598C-A1CD-4803-9046-6E701D5CD88B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A99AA882-DCA0-4F1F-8A57-9AA640B6CA03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6369,15 +6391,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{EBCB69A6-C64D-4BE8-9C07-0E53C070CD8C}" name="ErrorCode11" displayName="ErrorCode11" ref="K2:N14" totalsRowCount="1">
-  <autoFilter ref="K2:N13" xr:uid="{D5240800-A39B-4170-B586-F31A3108E3C4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F1110CBE-75E3-4F91-9E9F-58305AFC78B9}" name="ErrorCode7" displayName="ErrorCode7" ref="K2:N14" totalsRowCount="1">
+  <autoFilter ref="K2:N13" xr:uid="{6CEBD537-AAFC-43B3-839B-5AC35BCBF08B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{201BB9DD-3C17-4804-A8B8-E725CECEE9BB}" name="Error code"/>
-    <tableColumn id="2" xr3:uid="{E860FED4-4025-4DBF-AB56-CCFA3D8B0D70}" name="Description"/>
-    <tableColumn id="3" xr3:uid="{F1DDB5C4-65E3-416E-9637-AB9CFCE83F5E}" name="Total" totalsRowLabel="188"/>
-    <tableColumn id="4" xr3:uid="{7241D542-6A45-4716-A6E8-4D500B563F8E}" name="% of Total Errors" totalsRowFunction="custom" totalsRowDxfId="0" dataCellStyle="Percent">
-      <calculatedColumnFormula>ErrorCode11[[#This Row],[Total]]/ErrorCode11[[#Totals],[Total]]</calculatedColumnFormula>
-      <totalsRowFormula>SUM(ErrorCode11[% of Total Errors])</totalsRowFormula>
+    <tableColumn id="1" xr3:uid="{A1B13D0D-96DC-4CC7-83FB-404B84F6B4CB}" name="Error code"/>
+    <tableColumn id="2" xr3:uid="{8875EFAA-DB8C-4EF3-B636-5D17CAB43B6E}" name="Description"/>
+    <tableColumn id="3" xr3:uid="{B5C3CE92-A12D-4D5E-9B70-81372C6B6366}" name="Total" totalsRowLabel="188"/>
+    <tableColumn id="4" xr3:uid="{F4A22C7D-B2F3-4DF8-BA1C-0B789B948CF1}" name="% of Total Errors" totalsRowFunction="custom" totalsRowDxfId="4" dataCellStyle="Percent">
+      <calculatedColumnFormula>ErrorCode7[[#This Row],[Total]]/ErrorCode7[[#Totals],[Total]]</calculatedColumnFormula>
+      <totalsRowFormula>SUM(ErrorCode7[% of Total Errors])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6385,15 +6407,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D206F0F4-F36A-4CD3-8C4A-9075349DEC28}" name="ErrorCode" displayName="ErrorCode" ref="K2:N14" totalsRowCount="1">
-  <autoFilter ref="K2:N13" xr:uid="{26358E53-DD0D-4169-B665-52B4B814E22E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9887EA74-30BB-4863-9B1D-DDEAAA70DA1A}" name="ErrorCode" displayName="ErrorCode" ref="K2:N14" totalsRowCount="1">
+  <autoFilter ref="K2:N13" xr:uid="{FF4C394C-1025-43CC-A563-4B879E21BA93}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{AE478344-4F27-45C3-9F3D-F8825BF8A197}" name="Error code"/>
-    <tableColumn id="2" xr3:uid="{32438F50-DF00-438B-8894-8C5D6B511C73}" name="Description"/>
-    <tableColumn id="3" xr3:uid="{116C291B-AF03-49F8-B856-FDC397DD596A}" name="Total" totalsRowFunction="custom">
+    <tableColumn id="1" xr3:uid="{C788D75C-5DED-4542-A57E-FB4ABA10EF6C}" name="Error code"/>
+    <tableColumn id="2" xr3:uid="{265314A8-3787-4EA8-B027-D09968977EE4}" name="Description"/>
+    <tableColumn id="3" xr3:uid="{5270518B-726A-406C-8F55-E0D561DDEA26}" name="Total" totalsRowFunction="custom">
       <totalsRowFormula>SUM(ErrorCode[Total])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D69FB843-3F4F-43F0-901F-D1DB6FC2756D}" name="% of Total Errors" totalsRowFunction="custom" totalsRowDxfId="4" dataCellStyle="Percent">
+    <tableColumn id="4" xr3:uid="{879BD694-71CE-407F-A102-FEE93818167E}" name="% of Total Errors" totalsRowFunction="custom" totalsRowDxfId="3" dataCellStyle="Percent">
       <calculatedColumnFormula>ErrorCode[[#This Row],[Total]]/ErrorCode[[#Totals],[Total]]</calculatedColumnFormula>
       <totalsRowFormula>SUM(ErrorCode[% of Total Errors])</totalsRowFormula>
     </tableColumn>
@@ -6403,17 +6425,17 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{06756E05-DF6B-47AF-86A6-653A56432E4C}" name="ErrorCode8" displayName="ErrorCode8" ref="K2:N14" totalsRowCount="1">
-  <autoFilter ref="K2:N13" xr:uid="{9586492B-4B26-4610-A14F-D2C4BD5B39CE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7C1917FC-1771-4AAC-BF24-AF296A153D32}" name="ErrorCode4" displayName="ErrorCode4" ref="K2:N14" totalsRowCount="1">
+  <autoFilter ref="K2:N13" xr:uid="{DB9414FB-4A09-4B79-B642-B8B0EF95467E}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{591FC92A-287C-4D02-B229-F353BE8C4FF7}" name="Error code"/>
-    <tableColumn id="2" xr3:uid="{6B8A9623-9C23-4E92-9FAF-E6123F9872F0}" name="Description"/>
-    <tableColumn id="3" xr3:uid="{F235E710-4FC2-4EB9-AD9E-59C3726F55CA}" name="Total" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(ErrorCode8[Total])</totalsRowFormula>
+    <tableColumn id="1" xr3:uid="{05F3E594-F6E8-4B20-A7A4-D273596A8B66}" name="Error code"/>
+    <tableColumn id="2" xr3:uid="{9989890B-A7E6-4105-B44B-39F716039E1C}" name="Description"/>
+    <tableColumn id="3" xr3:uid="{224234AE-BE58-4EE5-840F-401129DCBA45}" name="Total" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(ErrorCode4[Total])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{1FA9AC78-68EA-4639-9CFA-16434E4ED08E}" name="% of Total Errors" totalsRowFunction="custom" totalsRowDxfId="3" dataCellStyle="Percent">
-      <calculatedColumnFormula>ErrorCode8[[#This Row],[Total]]/ErrorCode8[[#Totals],[Total]]</calculatedColumnFormula>
-      <totalsRowFormula>SUM(ErrorCode8[% of Total Errors])</totalsRowFormula>
+    <tableColumn id="4" xr3:uid="{F383A0F0-8714-4FF8-8543-D1595318F92E}" name="% of Total Errors" totalsRowFunction="custom" totalsRowDxfId="2" dataCellStyle="Percent">
+      <calculatedColumnFormula>ErrorCode4[[#This Row],[Total]]/ErrorCode4[[#Totals],[Total]]</calculatedColumnFormula>
+      <totalsRowFormula>SUM(ErrorCode4[% of Total Errors])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6421,17 +6443,17 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0C5A4F22-F43E-44D6-9D8D-43FF8A6209C0}" name="ErrorCode9" displayName="ErrorCode9" ref="K2:N14" totalsRowCount="1">
-  <autoFilter ref="K2:N13" xr:uid="{5DBF6E07-8350-44CB-9AE1-9ED50D1C1089}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F2355FB8-0018-4748-BF75-BEBCD26A3B34}" name="ErrorCode5" displayName="ErrorCode5" ref="K2:N14" totalsRowCount="1">
+  <autoFilter ref="K2:N13" xr:uid="{D3C4F67E-7A64-4827-B6E5-E7E8562BCCAA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{189CF8FB-4637-4A5A-822B-347D820A99A2}" name="Error code"/>
-    <tableColumn id="2" xr3:uid="{5FDC5013-A646-42CD-BE8E-0BC1BFB2EDAD}" name="Description"/>
-    <tableColumn id="3" xr3:uid="{1680B6A3-CA7A-4421-958E-5C3A6BCAC326}" name="Total" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(ErrorCode9[Total])</totalsRowFormula>
+    <tableColumn id="1" xr3:uid="{6E334CE1-9F69-4A1C-BE99-AF027A80CA1F}" name="Error code"/>
+    <tableColumn id="2" xr3:uid="{829C6178-A997-4B64-AA8F-46BCF8F8B73C}" name="Description"/>
+    <tableColumn id="3" xr3:uid="{5E1344D3-B076-444E-AF14-A48905971F4F}" name="Total" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(ErrorCode5[Total])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{818C2AD4-E7DA-41C4-B945-09487EF338FD}" name="% of Total Errors" totalsRowFunction="custom" totalsRowDxfId="2" dataCellStyle="Percent">
-      <calculatedColumnFormula>ErrorCode9[[#This Row],[Total]]/ErrorCode9[[#Totals],[Total]]</calculatedColumnFormula>
-      <totalsRowFormula>SUM(ErrorCode9[% of Total Errors])</totalsRowFormula>
+    <tableColumn id="4" xr3:uid="{643F28BE-9D48-46F0-B88C-A1BCD1973505}" name="% of Total Errors" totalsRowFunction="custom" totalsRowDxfId="1" dataCellStyle="Percent">
+      <calculatedColumnFormula>ErrorCode5[[#This Row],[Total]]/ErrorCode5[[#Totals],[Total]]</calculatedColumnFormula>
+      <totalsRowFormula>SUM(ErrorCode5[% of Total Errors])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6439,17 +6461,17 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{8EB76157-A685-4B2F-9012-2B070F4ABDCB}" name="ErrorCode10" displayName="ErrorCode10" ref="K2:N14" totalsRowCount="1">
-  <autoFilter ref="K2:N13" xr:uid="{EF096DEE-3E10-4BD2-9D0C-470701049CC9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{43E06458-B824-4340-8807-962F87E384D2}" name="ErrorCode6" displayName="ErrorCode6" ref="K2:N14" totalsRowCount="1">
+  <autoFilter ref="K2:N13" xr:uid="{72D9A441-CF58-4467-9145-B31F84AB45E3}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{1AD37761-61B1-4750-8E66-CF3EA53776A3}" name="Error code"/>
-    <tableColumn id="2" xr3:uid="{CCC035F0-A56A-44B3-8C0F-BD393ACAC390}" name="Description"/>
-    <tableColumn id="3" xr3:uid="{561654DC-C14B-49CD-8409-1A1768A62319}" name="Total" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(ErrorCode10[Total])</totalsRowFormula>
+    <tableColumn id="1" xr3:uid="{F5B5B8B0-B1F0-4EE4-B2F3-77A9FC7648B5}" name="Error code"/>
+    <tableColumn id="2" xr3:uid="{AD333218-E7DC-43E0-BF22-B4BEF2428274}" name="Description"/>
+    <tableColumn id="3" xr3:uid="{BEA58F6D-F48F-4EB2-A3DA-62CD7A49327C}" name="Total" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(ErrorCode6[Total])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C05D0CDB-9F1A-4AC4-8B36-DA5C2BCEDF05}" name="% of Total Errors" totalsRowFunction="custom" totalsRowDxfId="1" dataCellStyle="Percent">
-      <calculatedColumnFormula>ErrorCode10[[#This Row],[Total]]/ErrorCode10[[#Totals],[Total]]</calculatedColumnFormula>
-      <totalsRowFormula>SUM(ErrorCode10[% of Total Errors])</totalsRowFormula>
+    <tableColumn id="4" xr3:uid="{573C3A81-6F3F-428D-9BE4-823D116C5AA5}" name="% of Total Errors" totalsRowFunction="custom" totalsRowDxfId="0" dataCellStyle="Percent">
+      <calculatedColumnFormula>ErrorCode6[[#This Row],[Total]]/ErrorCode6[[#Totals],[Total]]</calculatedColumnFormula>
+      <totalsRowFormula>SUM(ErrorCode6[% of Total Errors])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6754,15 +6776,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500D4B20-C4CB-4368-B69B-968BC3A919A7}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="K2:N14"/>
+  <dimension ref="K2:T62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:N14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="17.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K2" t="s">
         <v>71</v>
       </c>
@@ -6775,8 +6800,14 @@
       <c r="N2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="3" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K3">
         <v>1</v>
       </c>
@@ -6787,11 +6818,25 @@
         <v>21</v>
       </c>
       <c r="N3" s="42">
-        <f>ErrorCode11[[#This Row],[Total]]/ErrorCode11[[#Totals],[Total]]</f>
+        <f>ErrorCode7[[#This Row],[Total]]/ErrorCode7[[#Totals],[Total]]</f>
         <v>0.11170212765957446</v>
       </c>
-    </row>
-    <row r="4" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>92</v>
+      </c>
+      <c r="S3">
+        <f>ErrorCode4[[#This Row],[Total]]</f>
+        <v>8</v>
+      </c>
+      <c r="T3" t="e">
+        <f>ErrorCode5[#Data]</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="4" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K4">
         <v>2</v>
       </c>
@@ -6802,11 +6847,25 @@
         <v>21</v>
       </c>
       <c r="N4" s="42">
-        <f>ErrorCode11[[#This Row],[Total]]/ErrorCode11[[#Totals],[Total]]</f>
+        <f>ErrorCode7[[#This Row],[Total]]/ErrorCode7[[#Totals],[Total]]</f>
         <v>0.11170212765957446</v>
       </c>
-    </row>
-    <row r="5" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>92</v>
+      </c>
+      <c r="S4">
+        <f>ErrorCode4[[#This Row],[Total]]</f>
+        <v>6</v>
+      </c>
+      <c r="T4" t="e">
+        <f>ErrorCode5[#Data]</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="5" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K5">
         <v>3</v>
       </c>
@@ -6817,11 +6876,25 @@
         <v>22</v>
       </c>
       <c r="N5" s="42">
-        <f>ErrorCode11[[#This Row],[Total]]/ErrorCode11[[#Totals],[Total]]</f>
+        <f>ErrorCode7[[#This Row],[Total]]/ErrorCode7[[#Totals],[Total]]</f>
         <v>0.11702127659574468</v>
       </c>
-    </row>
-    <row r="6" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="P5">
+        <v>2</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>92</v>
+      </c>
+      <c r="S5">
+        <f>ErrorCode4[[#This Row],[Total]]</f>
+        <v>9</v>
+      </c>
+      <c r="T5" t="e">
+        <f>ErrorCode5[#Data]</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="6" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K6">
         <v>4</v>
       </c>
@@ -6832,11 +6905,25 @@
         <v>22</v>
       </c>
       <c r="N6" s="42">
-        <f>ErrorCode11[[#This Row],[Total]]/ErrorCode11[[#Totals],[Total]]</f>
+        <f>ErrorCode7[[#This Row],[Total]]/ErrorCode7[[#Totals],[Total]]</f>
         <v>0.11702127659574468</v>
       </c>
-    </row>
-    <row r="7" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>92</v>
+      </c>
+      <c r="S6">
+        <f>ErrorCode4[[#This Row],[Total]]</f>
+        <v>9</v>
+      </c>
+      <c r="T6" t="e">
+        <f>ErrorCode5[#Data]</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="7" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K7">
         <v>5</v>
       </c>
@@ -6847,11 +6934,25 @@
         <v>29</v>
       </c>
       <c r="N7" s="42">
-        <f>ErrorCode11[[#This Row],[Total]]/ErrorCode11[[#Totals],[Total]]</f>
+        <f>ErrorCode7[[#This Row],[Total]]/ErrorCode7[[#Totals],[Total]]</f>
         <v>0.15425531914893617</v>
       </c>
-    </row>
-    <row r="8" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="P7">
+        <v>2</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>92</v>
+      </c>
+      <c r="S7">
+        <f>ErrorCode4[[#This Row],[Total]]</f>
+        <v>9</v>
+      </c>
+      <c r="T7" t="e">
+        <f>ErrorCode5[#Data]</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="8" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K8">
         <v>6</v>
       </c>
@@ -6862,11 +6963,25 @@
         <v>17</v>
       </c>
       <c r="N8" s="42">
-        <f>ErrorCode11[[#This Row],[Total]]/ErrorCode11[[#Totals],[Total]]</f>
+        <f>ErrorCode7[[#This Row],[Total]]/ErrorCode7[[#Totals],[Total]]</f>
         <v>9.0425531914893623E-2</v>
       </c>
-    </row>
-    <row r="9" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <v>2</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>92</v>
+      </c>
+      <c r="S8">
+        <f>ErrorCode4[[#This Row],[Total]]</f>
+        <v>9</v>
+      </c>
+      <c r="T8" t="e">
+        <f>ErrorCode5[#Data]</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="9" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K9">
         <v>7</v>
       </c>
@@ -6877,11 +6992,25 @@
         <v>16</v>
       </c>
       <c r="N9" s="42">
-        <f>ErrorCode11[[#This Row],[Total]]/ErrorCode11[[#Totals],[Total]]</f>
+        <f>ErrorCode7[[#This Row],[Total]]/ErrorCode7[[#Totals],[Total]]</f>
         <v>8.5106382978723402E-2</v>
       </c>
-    </row>
-    <row r="10" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="P9">
+        <v>2</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>92</v>
+      </c>
+      <c r="S9">
+        <f>ErrorCode4[[#This Row],[Total]]</f>
+        <v>9</v>
+      </c>
+      <c r="T9" t="e">
+        <f>ErrorCode5[#Data]</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="10" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K10">
         <v>8</v>
       </c>
@@ -6892,11 +7021,25 @@
         <v>16</v>
       </c>
       <c r="N10" s="42">
-        <f>ErrorCode11[[#This Row],[Total]]/ErrorCode11[[#Totals],[Total]]</f>
+        <f>ErrorCode7[[#This Row],[Total]]/ErrorCode7[[#Totals],[Total]]</f>
         <v>8.5106382978723402E-2</v>
       </c>
-    </row>
-    <row r="11" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="P10">
+        <v>3</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>92</v>
+      </c>
+      <c r="S10">
+        <f>ErrorCode4[[#This Row],[Total]]</f>
+        <v>9</v>
+      </c>
+      <c r="T10" t="e">
+        <f>ErrorCode5[#Data]</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="11" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K11">
         <v>9</v>
       </c>
@@ -6907,11 +7050,25 @@
         <v>16</v>
       </c>
       <c r="N11" s="42">
-        <f>ErrorCode11[[#This Row],[Total]]/ErrorCode11[[#Totals],[Total]]</f>
+        <f>ErrorCode7[[#This Row],[Total]]/ErrorCode7[[#Totals],[Total]]</f>
         <v>8.5106382978723402E-2</v>
       </c>
-    </row>
-    <row r="12" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="P11">
+        <v>3</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>92</v>
+      </c>
+      <c r="S11">
+        <f>ErrorCode4[[#This Row],[Total]]</f>
+        <v>9</v>
+      </c>
+      <c r="T11" t="e">
+        <f>ErrorCode5[#Data]</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="12" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K12">
         <v>10</v>
       </c>
@@ -6922,11 +7079,25 @@
         <v>7</v>
       </c>
       <c r="N12" s="42">
-        <f>ErrorCode11[[#This Row],[Total]]/ErrorCode11[[#Totals],[Total]]</f>
+        <f>ErrorCode7[[#This Row],[Total]]/ErrorCode7[[#Totals],[Total]]</f>
         <v>3.7234042553191488E-2</v>
       </c>
-    </row>
-    <row r="13" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="P12">
+        <v>3</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>92</v>
+      </c>
+      <c r="S12">
+        <f>ErrorCode4[[#This Row],[Total]]</f>
+        <v>0</v>
+      </c>
+      <c r="T12" t="e">
+        <f>ErrorCode5[#Data]</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="13" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K13">
         <v>11</v>
       </c>
@@ -6934,17 +7105,429 @@
         <v>89</v>
       </c>
       <c r="N13" s="42">
-        <f>ErrorCode11[[#This Row],[Total]]/ErrorCode11[[#Totals],[Total]]</f>
+        <f>ErrorCode7[[#This Row],[Total]]/ErrorCode7[[#Totals],[Total]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="P13">
+        <v>3</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>92</v>
+      </c>
+      <c r="S13">
+        <f>ErrorCode4[[#This Row],[Total]]</f>
+        <v>0</v>
+      </c>
+      <c r="T13" t="e">
+        <f>ErrorCode5[#Data]</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="14" spans="11:20" x14ac:dyDescent="0.25">
       <c r="M14" t="s">
         <v>91</v>
       </c>
       <c r="N14" s="43">
-        <f>SUM(ErrorCode11[% of Total Errors])</f>
+        <f>SUM(ErrorCode7[% of Total Errors])</f>
         <v>0.99468085106382986</v>
+      </c>
+      <c r="P14" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="P15" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="P16">
+        <v>4</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="P17" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="P18" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L19" t="e">
+        <f>ErrorCode4[Error code]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P19">
+        <v>5</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L20" t="str">
+        <f>ErrorCode7[[#Headers],[Total]]</f>
+        <v>Total</v>
+      </c>
+      <c r="P20" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="P21" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="P22" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="P28" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="P29" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="P30" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="P31" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="P32" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P33" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P34" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P35">
+        <v>5</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P36">
+        <v>5</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P37">
+        <v>5</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P38">
+        <v>5</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P39">
+        <v>5</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P40">
+        <v>5</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P41">
+        <v>5</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P42">
+        <v>5</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P43">
+        <v>5</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P44">
+        <v>5</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P45">
+        <v>5</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P46">
+        <v>5</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P47" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P48">
+        <v>5</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P49">
+        <v>5</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P50" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P51" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="52" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P52" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P53">
+        <v>4</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P54">
+        <v>4</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P55">
+        <v>4</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="56" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P56">
+        <v>4</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P57" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P58">
+        <v>4</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="59" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P59">
+        <v>1</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P60" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="61" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P61">
+        <v>4</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="62" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P62">
+        <v>1</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -8702,7 +9285,7 @@
   <dimension ref="A1:N133"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:N14"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8784,7 +9367,7 @@
         <v>8</v>
       </c>
       <c r="N3" s="42">
-        <f>ErrorCode8[[#This Row],[Total]]/ErrorCode8[[#Totals],[Total]]</f>
+        <f>ErrorCode4[[#This Row],[Total]]/ErrorCode4[[#Totals],[Total]]</f>
         <v>0.1038961038961039</v>
       </c>
     </row>
@@ -8821,7 +9404,7 @@
         <v>6</v>
       </c>
       <c r="N4" s="42">
-        <f>ErrorCode8[[#This Row],[Total]]/ErrorCode8[[#Totals],[Total]]</f>
+        <f>ErrorCode4[[#This Row],[Total]]/ErrorCode4[[#Totals],[Total]]</f>
         <v>7.792207792207792E-2</v>
       </c>
     </row>
@@ -8858,7 +9441,7 @@
         <v>9</v>
       </c>
       <c r="N5" s="42">
-        <f>ErrorCode8[[#This Row],[Total]]/ErrorCode8[[#Totals],[Total]]</f>
+        <f>ErrorCode4[[#This Row],[Total]]/ErrorCode4[[#Totals],[Total]]</f>
         <v>0.11688311688311688</v>
       </c>
     </row>
@@ -8895,7 +9478,7 @@
         <v>9</v>
       </c>
       <c r="N6" s="42">
-        <f>ErrorCode8[[#This Row],[Total]]/ErrorCode8[[#Totals],[Total]]</f>
+        <f>ErrorCode4[[#This Row],[Total]]/ErrorCode4[[#Totals],[Total]]</f>
         <v>0.11688311688311688</v>
       </c>
     </row>
@@ -8932,7 +9515,7 @@
         <v>9</v>
       </c>
       <c r="N7" s="42">
-        <f>ErrorCode8[[#This Row],[Total]]/ErrorCode8[[#Totals],[Total]]</f>
+        <f>ErrorCode4[[#This Row],[Total]]/ErrorCode4[[#Totals],[Total]]</f>
         <v>0.11688311688311688</v>
       </c>
     </row>
@@ -8969,7 +9552,7 @@
         <v>9</v>
       </c>
       <c r="N8" s="42">
-        <f>ErrorCode8[[#This Row],[Total]]/ErrorCode8[[#Totals],[Total]]</f>
+        <f>ErrorCode4[[#This Row],[Total]]/ErrorCode4[[#Totals],[Total]]</f>
         <v>0.11688311688311688</v>
       </c>
     </row>
@@ -9006,7 +9589,7 @@
         <v>9</v>
       </c>
       <c r="N9" s="42">
-        <f>ErrorCode8[[#This Row],[Total]]/ErrorCode8[[#Totals],[Total]]</f>
+        <f>ErrorCode4[[#This Row],[Total]]/ErrorCode4[[#Totals],[Total]]</f>
         <v>0.11688311688311688</v>
       </c>
     </row>
@@ -9043,7 +9626,7 @@
         <v>9</v>
       </c>
       <c r="N10" s="42">
-        <f>ErrorCode8[[#This Row],[Total]]/ErrorCode8[[#Totals],[Total]]</f>
+        <f>ErrorCode4[[#This Row],[Total]]/ErrorCode4[[#Totals],[Total]]</f>
         <v>0.11688311688311688</v>
       </c>
     </row>
@@ -9080,7 +9663,7 @@
         <v>9</v>
       </c>
       <c r="N11" s="42">
-        <f>ErrorCode8[[#This Row],[Total]]/ErrorCode8[[#Totals],[Total]]</f>
+        <f>ErrorCode4[[#This Row],[Total]]/ErrorCode4[[#Totals],[Total]]</f>
         <v>0.11688311688311688</v>
       </c>
     </row>
@@ -9101,7 +9684,7 @@
       </c>
       <c r="M12"/>
       <c r="N12" s="42">
-        <f>ErrorCode8[[#This Row],[Total]]/ErrorCode8[[#Totals],[Total]]</f>
+        <f>ErrorCode4[[#This Row],[Total]]/ErrorCode4[[#Totals],[Total]]</f>
         <v>0</v>
       </c>
     </row>
@@ -9136,7 +9719,7 @@
       </c>
       <c r="M13"/>
       <c r="N13" s="42">
-        <f>ErrorCode8[[#This Row],[Total]]/ErrorCode8[[#Totals],[Total]]</f>
+        <f>ErrorCode4[[#This Row],[Total]]/ErrorCode4[[#Totals],[Total]]</f>
         <v>0</v>
       </c>
     </row>
@@ -9166,11 +9749,11 @@
       <c r="K14"/>
       <c r="L14"/>
       <c r="M14">
-        <f>SUM(ErrorCode8[Total])</f>
+        <f>SUM(ErrorCode4[Total])</f>
         <v>77</v>
       </c>
       <c r="N14" s="43">
-        <f>SUM(ErrorCode8[% of Total Errors])</f>
+        <f>SUM(ErrorCode4[% of Total Errors])</f>
         <v>1</v>
       </c>
     </row>
@@ -10510,7 +11093,7 @@
         <v>4</v>
       </c>
       <c r="N3" s="42">
-        <f>ErrorCode9[[#This Row],[Total]]/ErrorCode9[[#Totals],[Total]]</f>
+        <f>ErrorCode5[[#This Row],[Total]]/ErrorCode5[[#Totals],[Total]]</f>
         <v>0.08</v>
       </c>
     </row>
@@ -10547,7 +11130,7 @@
         <v>4</v>
       </c>
       <c r="N4" s="42">
-        <f>ErrorCode9[[#This Row],[Total]]/ErrorCode9[[#Totals],[Total]]</f>
+        <f>ErrorCode5[[#This Row],[Total]]/ErrorCode5[[#Totals],[Total]]</f>
         <v>0.08</v>
       </c>
     </row>
@@ -10584,7 +11167,7 @@
         <v>4</v>
       </c>
       <c r="N5" s="42">
-        <f>ErrorCode9[[#This Row],[Total]]/ErrorCode9[[#Totals],[Total]]</f>
+        <f>ErrorCode5[[#This Row],[Total]]/ErrorCode5[[#Totals],[Total]]</f>
         <v>0.08</v>
       </c>
     </row>
@@ -10621,7 +11204,7 @@
         <v>4</v>
       </c>
       <c r="N6" s="42">
-        <f>ErrorCode9[[#This Row],[Total]]/ErrorCode9[[#Totals],[Total]]</f>
+        <f>ErrorCode5[[#This Row],[Total]]/ErrorCode5[[#Totals],[Total]]</f>
         <v>0.08</v>
       </c>
     </row>
@@ -10658,7 +11241,7 @@
         <v>14</v>
       </c>
       <c r="N7" s="42">
-        <f>ErrorCode9[[#This Row],[Total]]/ErrorCode9[[#Totals],[Total]]</f>
+        <f>ErrorCode5[[#This Row],[Total]]/ErrorCode5[[#Totals],[Total]]</f>
         <v>0.28000000000000003</v>
       </c>
     </row>
@@ -10695,7 +11278,7 @@
         <v>4</v>
       </c>
       <c r="N8" s="42">
-        <f>ErrorCode9[[#This Row],[Total]]/ErrorCode9[[#Totals],[Total]]</f>
+        <f>ErrorCode5[[#This Row],[Total]]/ErrorCode5[[#Totals],[Total]]</f>
         <v>0.08</v>
       </c>
     </row>
@@ -10732,7 +11315,7 @@
         <v>4</v>
       </c>
       <c r="N9" s="42">
-        <f>ErrorCode9[[#This Row],[Total]]/ErrorCode9[[#Totals],[Total]]</f>
+        <f>ErrorCode5[[#This Row],[Total]]/ErrorCode5[[#Totals],[Total]]</f>
         <v>0.08</v>
       </c>
     </row>
@@ -10769,7 +11352,7 @@
         <v>4</v>
       </c>
       <c r="N10" s="42">
-        <f>ErrorCode9[[#This Row],[Total]]/ErrorCode9[[#Totals],[Total]]</f>
+        <f>ErrorCode5[[#This Row],[Total]]/ErrorCode5[[#Totals],[Total]]</f>
         <v>0.08</v>
       </c>
     </row>
@@ -10806,7 +11389,7 @@
         <v>4</v>
       </c>
       <c r="N11" s="42">
-        <f>ErrorCode9[[#This Row],[Total]]/ErrorCode9[[#Totals],[Total]]</f>
+        <f>ErrorCode5[[#This Row],[Total]]/ErrorCode5[[#Totals],[Total]]</f>
         <v>0.08</v>
       </c>
     </row>
@@ -10831,7 +11414,7 @@
         <v>4</v>
       </c>
       <c r="N12" s="42">
-        <f>ErrorCode9[[#This Row],[Total]]/ErrorCode9[[#Totals],[Total]]</f>
+        <f>ErrorCode5[[#This Row],[Total]]/ErrorCode5[[#Totals],[Total]]</f>
         <v>0.08</v>
       </c>
     </row>
@@ -10862,7 +11445,7 @@
       </c>
       <c r="M13"/>
       <c r="N13" s="42">
-        <f>ErrorCode9[[#This Row],[Total]]/ErrorCode9[[#Totals],[Total]]</f>
+        <f>ErrorCode5[[#This Row],[Total]]/ErrorCode5[[#Totals],[Total]]</f>
         <v>0</v>
       </c>
     </row>
@@ -10888,11 +11471,11 @@
       <c r="K14"/>
       <c r="L14"/>
       <c r="M14">
-        <f>SUM(ErrorCode9[Total])</f>
+        <f>SUM(ErrorCode5[Total])</f>
         <v>50</v>
       </c>
       <c r="N14" s="43">
-        <f>SUM(ErrorCode9[% of Total Errors])</f>
+        <f>SUM(ErrorCode5[% of Total Errors])</f>
         <v>0.99999999999999989</v>
       </c>
     </row>
@@ -12183,7 +12766,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:N133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K2" sqref="K2:N14"/>
     </sheetView>
   </sheetViews>
@@ -12266,7 +12849,7 @@
         <v>5</v>
       </c>
       <c r="N3" s="42">
-        <f>ErrorCode10[[#This Row],[Total]]/ErrorCode10[[#Totals],[Total]]</f>
+        <f>ErrorCode6[[#This Row],[Total]]/ErrorCode6[[#Totals],[Total]]</f>
         <v>0.14285714285714285</v>
       </c>
     </row>
@@ -12303,7 +12886,7 @@
         <v>3</v>
       </c>
       <c r="N4" s="42">
-        <f>ErrorCode10[[#This Row],[Total]]/ErrorCode10[[#Totals],[Total]]</f>
+        <f>ErrorCode6[[#This Row],[Total]]/ErrorCode6[[#Totals],[Total]]</f>
         <v>8.5714285714285715E-2</v>
       </c>
     </row>
@@ -12340,7 +12923,7 @@
         <v>3</v>
       </c>
       <c r="N5" s="42">
-        <f>ErrorCode10[[#This Row],[Total]]/ErrorCode10[[#Totals],[Total]]</f>
+        <f>ErrorCode6[[#This Row],[Total]]/ErrorCode6[[#Totals],[Total]]</f>
         <v>8.5714285714285715E-2</v>
       </c>
     </row>
@@ -12377,7 +12960,7 @@
         <v>6</v>
       </c>
       <c r="N6" s="42">
-        <f>ErrorCode10[[#This Row],[Total]]/ErrorCode10[[#Totals],[Total]]</f>
+        <f>ErrorCode6[[#This Row],[Total]]/ErrorCode6[[#Totals],[Total]]</f>
         <v>0.17142857142857143</v>
       </c>
     </row>
@@ -12414,7 +12997,7 @@
         <v>3</v>
       </c>
       <c r="N7" s="42">
-        <f>ErrorCode10[[#This Row],[Total]]/ErrorCode10[[#Totals],[Total]]</f>
+        <f>ErrorCode6[[#This Row],[Total]]/ErrorCode6[[#Totals],[Total]]</f>
         <v>8.5714285714285715E-2</v>
       </c>
     </row>
@@ -12451,7 +13034,7 @@
         <v>3</v>
       </c>
       <c r="N8" s="42">
-        <f>ErrorCode10[[#This Row],[Total]]/ErrorCode10[[#Totals],[Total]]</f>
+        <f>ErrorCode6[[#This Row],[Total]]/ErrorCode6[[#Totals],[Total]]</f>
         <v>8.5714285714285715E-2</v>
       </c>
     </row>
@@ -12488,7 +13071,7 @@
         <v>3</v>
       </c>
       <c r="N9" s="42">
-        <f>ErrorCode10[[#This Row],[Total]]/ErrorCode10[[#Totals],[Total]]</f>
+        <f>ErrorCode6[[#This Row],[Total]]/ErrorCode6[[#Totals],[Total]]</f>
         <v>8.5714285714285715E-2</v>
       </c>
     </row>
@@ -12525,7 +13108,7 @@
         <v>3</v>
       </c>
       <c r="N10" s="42">
-        <f>ErrorCode10[[#This Row],[Total]]/ErrorCode10[[#Totals],[Total]]</f>
+        <f>ErrorCode6[[#This Row],[Total]]/ErrorCode6[[#Totals],[Total]]</f>
         <v>8.5714285714285715E-2</v>
       </c>
     </row>
@@ -12562,7 +13145,7 @@
         <v>3</v>
       </c>
       <c r="N11" s="42">
-        <f>ErrorCode10[[#This Row],[Total]]/ErrorCode10[[#Totals],[Total]]</f>
+        <f>ErrorCode6[[#This Row],[Total]]/ErrorCode6[[#Totals],[Total]]</f>
         <v>8.5714285714285715E-2</v>
       </c>
     </row>
@@ -12585,7 +13168,7 @@
         <v>3</v>
       </c>
       <c r="N12" s="42">
-        <f>ErrorCode10[[#This Row],[Total]]/ErrorCode10[[#Totals],[Total]]</f>
+        <f>ErrorCode6[[#This Row],[Total]]/ErrorCode6[[#Totals],[Total]]</f>
         <v>8.5714285714285715E-2</v>
       </c>
     </row>
@@ -12606,7 +13189,7 @@
       </c>
       <c r="M13"/>
       <c r="N13" s="42">
-        <f>ErrorCode10[[#This Row],[Total]]/ErrorCode10[[#Totals],[Total]]</f>
+        <f>ErrorCode6[[#This Row],[Total]]/ErrorCode6[[#Totals],[Total]]</f>
         <v>0</v>
       </c>
     </row>
@@ -12636,11 +13219,11 @@
       <c r="K14"/>
       <c r="L14"/>
       <c r="M14">
-        <f>SUM(ErrorCode10[Total])</f>
+        <f>SUM(ErrorCode6[Total])</f>
         <v>35</v>
       </c>
       <c r="N14" s="43">
-        <f>SUM(ErrorCode10[% of Total Errors])</f>
+        <f>SUM(ErrorCode6[% of Total Errors])</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>